<commit_message>
enhance: drilling dashboard KPI accuracy and cost allocation processing
- Add Deepwater Invictus drilling LC numbers (10140, 10133) to resolve June 2025 tonnage calculations
- Remove cost-per-ton KPI and replace with cost-per-hour for more accurate vessel utilization metrics
- Enhance cost allocation processor with explicit rig reference prioritization over text-based matching
- Add numeric MM-YY date format parsing (06-25, 12-24) for improved month-year processing
- Update dashboard hero metrics to show fluid volume and vessel visits instead of cargo tonnage
- Improve LC-to-location mapping with better debugging for Thunder Horse, Mad Dog, and Deepwater Invictus
- Refactor drilling metrics calculation to focus on operational efficiency rather than cargo weight

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/excel-data/excel-files/Cost Allocation.xlsx
+++ b/excel-data/excel-files/Cost Allocation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10720"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nealasmothers/Downloads/logisticsdashboard/excel-data/excel-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BECA04D-118E-2B42-8536-0B5B48F2DEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B002705-2D2C-7144-B2E7-C304B5609462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="920" windowWidth="34240" windowHeight="21260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2214" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="321">
   <si>
     <t>16THR0101M</t>
   </si>
@@ -937,150 +937,30 @@
     <t>04-25</t>
   </si>
   <si>
-    <t>10101</t>
-  </si>
-  <si>
-    <t>25.874</t>
-  </si>
-  <si>
-    <t>10133</t>
-  </si>
-  <si>
-    <t>65.502</t>
-  </si>
-  <si>
-    <t>10134</t>
-  </si>
-  <si>
-    <t>.251</t>
-  </si>
-  <si>
-    <t>10138</t>
-  </si>
-  <si>
-    <t>7.736</t>
-  </si>
-  <si>
-    <t>10139</t>
-  </si>
-  <si>
-    <t>40.106</t>
-  </si>
-  <si>
-    <t>9359</t>
-  </si>
-  <si>
-    <t>15.458</t>
-  </si>
-  <si>
-    <t>9360</t>
-  </si>
-  <si>
-    <t>22.469</t>
-  </si>
-  <si>
-    <t>9361</t>
-  </si>
-  <si>
-    <t>18.072</t>
-  </si>
-  <si>
-    <t>9364</t>
-  </si>
-  <si>
-    <t>1.249</t>
-  </si>
-  <si>
-    <t>10115</t>
-  </si>
-  <si>
     <t>H-S1E00EXP98-EX-D1</t>
   </si>
   <si>
     <t>Ocean Blackhornet / Penguin Exploration Well Long Leads:Penguin Long Leads materials/inventory</t>
   </si>
   <si>
-    <t>.257</t>
-  </si>
-  <si>
-    <t>10116</t>
-  </si>
-  <si>
-    <t>57.445</t>
-  </si>
-  <si>
-    <t>10137</t>
-  </si>
-  <si>
-    <t>36.703</t>
-  </si>
-  <si>
-    <t>10092</t>
-  </si>
-  <si>
-    <t>.731</t>
-  </si>
-  <si>
-    <t>9358</t>
-  </si>
-  <si>
-    <t>7.351</t>
-  </si>
-  <si>
-    <t>9984</t>
-  </si>
-  <si>
-    <t>7.404</t>
-  </si>
-  <si>
-    <t>9999</t>
-  </si>
-  <si>
-    <t>8.732</t>
-  </si>
-  <si>
-    <t>10055</t>
-  </si>
-  <si>
     <t>H-S1DW0ATL3V-EX-D1-DF</t>
   </si>
   <si>
     <t>IceMax / ATL DC104 Water Injector Drilling: ATL DC104 WI - Drill Well - DRILL</t>
   </si>
   <si>
-    <t>32.679</t>
-  </si>
-  <si>
-    <t>10131</t>
-  </si>
-  <si>
     <t>H-S1DW0THR92-EX-D1-DU</t>
   </si>
   <si>
     <t>C-Constructor / MC777-2 (NPi22) Drilling Long Lead: MC 777-2 Drill Well - LLs intangible</t>
   </si>
   <si>
-    <t>.033</t>
-  </si>
-  <si>
-    <t>10124</t>
-  </si>
-  <si>
     <t>H-S1DW0MAD5X-EX-D1-DF</t>
   </si>
   <si>
     <t>Ocean Blacklion / MD2 GC826-13 MD122 (SP3) - Drill Long Le: MD2 GC826-13 MD122 (SP3) Producer Drilli</t>
   </si>
   <si>
-    <t>28.261</t>
-  </si>
-  <si>
-    <t>10114</t>
-  </si>
-  <si>
-    <t>.35</t>
-  </si>
-  <si>
     <t>05-25</t>
   </si>
   <si>
@@ -1090,67 +970,16 @@
     <t>Stena IceMAX</t>
   </si>
   <si>
-    <t>19.451</t>
-  </si>
-  <si>
-    <t>63.655</t>
-  </si>
-  <si>
-    <t>9.681</t>
-  </si>
-  <si>
-    <t>61.058</t>
-  </si>
-  <si>
-    <t>47.463</t>
-  </si>
-  <si>
-    <t>41.618</t>
-  </si>
-  <si>
-    <t>12.316</t>
-  </si>
-  <si>
-    <t>10140</t>
-  </si>
-  <si>
     <t>H-S1DW0MAD5V-EX-D1-CF</t>
   </si>
   <si>
     <t>Deepwater Invictus / Argos SWX4 BP01 (GC 868-1) Producer Comp: Mad Dog Compl Well - COMPLETE LL</t>
   </si>
   <si>
-    <t>26.346</t>
-  </si>
-  <si>
-    <t>20.596</t>
-  </si>
-  <si>
-    <t>10.041</t>
-  </si>
-  <si>
-    <t>12.884</t>
-  </si>
-  <si>
-    <t>8.173</t>
-  </si>
-  <si>
-    <t>7.548</t>
-  </si>
-  <si>
-    <t>10130</t>
-  </si>
-  <si>
     <t>H-S1DC1MAD5E-EX-I0-T0-E5</t>
   </si>
   <si>
     <t>Olympic Challenger / Argos Southwest Extension Fabrication AF: ASWX - Installation-System Tie-In</t>
-  </si>
-  <si>
-    <t>.565</t>
-  </si>
-  <si>
-    <t>.209</t>
   </si>
   <si>
     <t>06-25</t>
@@ -1301,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1333,19 +1162,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1353,6 +1176,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1969,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A329" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E358" sqref="E358"/>
+    <sheetView tabSelected="1" topLeftCell="A341" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C334" sqref="C334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2077,7 +1903,7 @@
         <v>31.177</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>289</v>
@@ -2623,7 +2449,7 @@
         <v>60.441000000000003</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>290</v>
@@ -3169,7 +2995,7 @@
         <v>62.722000000000001</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>291</v>
@@ -3611,7 +3437,7 @@
         <v>42.377000000000002</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F63" s="11" t="s">
         <v>292</v>
@@ -3741,7 +3567,7 @@
         <v>19.596</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F68" s="11" t="s">
         <v>292</v>
@@ -4105,7 +3931,7 @@
         <v>62.593000000000004</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F82" s="11" t="s">
         <v>293</v>
@@ -4677,7 +4503,7 @@
         <v>56.954000000000001</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F104" s="11" t="s">
         <v>294</v>
@@ -5301,7 +5127,7 @@
         <v>52.415999999999997</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F128" s="11" t="s">
         <v>295</v>
@@ -5405,7 +5231,7 @@
         <v>2.617</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F132" s="11" t="s">
         <v>295</v>
@@ -5509,7 +5335,7 @@
         <v>95.087999999999994</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F136" s="11" t="s">
         <v>296</v>
@@ -5873,7 +5699,7 @@
         <v>3.242</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F150" s="11" t="s">
         <v>296</v>
@@ -5899,7 +5725,7 @@
         <v>1.036</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F151" s="11" t="s">
         <v>296</v>
@@ -6003,7 +5829,7 @@
         <v>33.215000000000003</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F155" s="11" t="s">
         <v>297</v>
@@ -6367,7 +6193,7 @@
         <v>40.658999999999999</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F169" s="11" t="s">
         <v>297</v>
@@ -6393,7 +6219,7 @@
         <v>2.548</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F170" s="11" t="s">
         <v>297</v>
@@ -6627,7 +6453,7 @@
         <v>67.941999999999993</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F179" s="11" t="s">
         <v>298</v>
@@ -7147,7 +6973,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F199" s="11" t="s">
         <v>298</v>
@@ -7251,7 +7077,7 @@
         <v>27.385999999999999</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F203" s="11" t="s">
         <v>299</v>
@@ -7849,7 +7675,7 @@
         <v>29.285</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F226" s="11" t="s">
         <v>300</v>
@@ -7875,7 +7701,7 @@
         <v>19.824000000000002</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F227" s="11" t="s">
         <v>300</v>
@@ -8317,7 +8143,7 @@
         <v>0.72499999999999998</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F244" s="11" t="s">
         <v>300</v>
@@ -8369,7 +8195,7 @@
         <v>3.593</v>
       </c>
       <c r="E246" s="5" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F246" s="11" t="s">
         <v>301</v>
@@ -8473,7 +8299,7 @@
         <v>43.456000000000003</v>
       </c>
       <c r="E250" s="5" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F250" s="11" t="s">
         <v>301</v>
@@ -8941,7 +8767,7 @@
         <v>19.37</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F268" s="11" t="s">
         <v>302</v>
@@ -8967,7 +8793,7 @@
         <v>40.31</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F269" s="11" t="s">
         <v>302</v>
@@ -9487,7 +9313,7 @@
         <v>43.725000000000001</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F289" s="11" t="s">
         <v>303</v>
@@ -9981,7 +9807,7 @@
         <v>14.464</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F308" s="11" t="s">
         <v>304</v>
@@ -10085,7 +9911,7 @@
         <v>43.155999999999999</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F312" s="11" t="s">
         <v>304</v>
@@ -10358,8 +10184,8 @@
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A323" s="1" t="s">
-        <v>305</v>
+      <c r="A323" s="19">
+        <v>10101</v>
       </c>
       <c r="B323" s="1" t="s">
         <v>255</v>
@@ -10367,25 +10193,25 @@
       <c r="C323" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D323" s="1" t="s">
-        <v>306</v>
+      <c r="D323" s="19">
+        <v>25.873999999999999</v>
       </c>
       <c r="E323" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F323" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>354</v>
+        <v>314</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A324" s="1" t="s">
-        <v>307</v>
+      <c r="A324" s="19">
+        <v>10133</v>
       </c>
       <c r="B324" s="1" t="s">
         <v>275</v>
@@ -10393,14 +10219,14 @@
       <c r="C324" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D324" s="1" t="s">
-        <v>308</v>
+      <c r="D324" s="19">
+        <v>65.501999999999995</v>
       </c>
       <c r="E324" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F324" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G324" s="1" t="s">
         <v>282</v>
@@ -10410,8 +10236,8 @@
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A325" s="1" t="s">
-        <v>309</v>
+      <c r="A325" s="19">
+        <v>10134</v>
       </c>
       <c r="B325" s="1" t="s">
         <v>259</v>
@@ -10419,14 +10245,14 @@
       <c r="C325" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D325" s="1" t="s">
-        <v>310</v>
+      <c r="D325" s="19">
+        <v>0.251</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F325" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G325" s="1" t="s">
         <v>288</v>
@@ -10436,8 +10262,8 @@
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A326" s="1" t="s">
-        <v>311</v>
+      <c r="A326" s="19">
+        <v>10138</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>269</v>
@@ -10445,14 +10271,14 @@
       <c r="C326" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D326" s="1" t="s">
-        <v>312</v>
+      <c r="D326" s="19">
+        <v>7.7359999999999998</v>
       </c>
       <c r="E326" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F326" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G326" s="1" t="s">
         <v>284</v>
@@ -10462,8 +10288,8 @@
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A327" s="1" t="s">
-        <v>313</v>
+      <c r="A327" s="19">
+        <v>10139</v>
       </c>
       <c r="B327" s="1" t="s">
         <v>271</v>
@@ -10471,14 +10297,14 @@
       <c r="C327" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D327" s="1" t="s">
-        <v>314</v>
+      <c r="D327" s="19">
+        <v>40.106000000000002</v>
       </c>
       <c r="E327" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F327" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G327" s="1" t="s">
         <v>285</v>
@@ -10488,8 +10314,8 @@
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A328" s="1" t="s">
-        <v>315</v>
+      <c r="A328" s="19">
+        <v>9359</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>30</v>
@@ -10497,14 +10323,14 @@
       <c r="C328" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D328" s="1" t="s">
-        <v>316</v>
+      <c r="D328" s="19">
+        <v>15.458</v>
       </c>
       <c r="E328" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F328" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G328" s="1" t="s">
         <v>281</v>
@@ -10514,8 +10340,8 @@
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A329" s="1" t="s">
-        <v>317</v>
+      <c r="A329" s="19">
+        <v>9360</v>
       </c>
       <c r="B329" s="1" t="s">
         <v>0</v>
@@ -10523,14 +10349,14 @@
       <c r="C329" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D329" s="1" t="s">
-        <v>318</v>
+      <c r="D329" s="19">
+        <v>22.469000000000001</v>
       </c>
       <c r="E329" s="1" t="s">
         <v>105</v>
       </c>
       <c r="F329" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G329" s="1" t="s">
         <v>281</v>
@@ -10540,8 +10366,8 @@
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A330" s="1" t="s">
-        <v>319</v>
+      <c r="A330" s="19">
+        <v>9361</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>21</v>
@@ -10549,14 +10375,14 @@
       <c r="C330" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D330" s="1" t="s">
-        <v>320</v>
+      <c r="D330" s="19">
+        <v>18.071999999999999</v>
       </c>
       <c r="E330" s="1" t="s">
         <v>110</v>
       </c>
       <c r="F330" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G330" s="1" t="s">
         <v>281</v>
@@ -10566,8 +10392,8 @@
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A331" s="1" t="s">
-        <v>321</v>
+      <c r="A331" s="19">
+        <v>9364</v>
       </c>
       <c r="B331" s="1" t="s">
         <v>32</v>
@@ -10575,14 +10401,14 @@
       <c r="C331" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D331" s="1" t="s">
-        <v>322</v>
+      <c r="D331" s="19">
+        <v>1.2490000000000001</v>
       </c>
       <c r="E331" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F331" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G331" s="1" t="s">
         <v>281</v>
@@ -10592,23 +10418,23 @@
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A332" s="1" t="s">
-        <v>323</v>
+      <c r="A332" s="19">
+        <v>10115</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>324</v>
+        <v>305</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D332" s="1" t="s">
-        <v>326</v>
+        <v>306</v>
+      </c>
+      <c r="D332" s="19">
+        <v>0.25700000000000001</v>
       </c>
       <c r="E332" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F332" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G332" s="1" t="s">
         <v>282</v>
@@ -10618,8 +10444,8 @@
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A333" s="1" t="s">
-        <v>327</v>
+      <c r="A333" s="19">
+        <v>10116</v>
       </c>
       <c r="B333" s="1" t="s">
         <v>248</v>
@@ -10627,14 +10453,14 @@
       <c r="C333" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D333" s="1" t="s">
-        <v>328</v>
+      <c r="D333" s="19">
+        <v>57.445</v>
       </c>
       <c r="E333" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F333" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G333" s="1" t="s">
         <v>282</v>
@@ -10644,8 +10470,8 @@
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A334" s="1" t="s">
-        <v>329</v>
+      <c r="A334" s="19">
+        <v>10137</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>277</v>
@@ -10653,14 +10479,14 @@
       <c r="C334" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D334" s="1" t="s">
-        <v>330</v>
+      <c r="D334" s="19">
+        <v>36.703000000000003</v>
       </c>
       <c r="E334" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F334" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G334" s="1" t="s">
         <v>285</v>
@@ -10670,8 +10496,8 @@
       </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A335" s="1" t="s">
-        <v>331</v>
+      <c r="A335" s="19">
+        <v>10092</v>
       </c>
       <c r="B335" s="1" t="s">
         <v>205</v>
@@ -10679,14 +10505,14 @@
       <c r="C335" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D335" s="1" t="s">
-        <v>332</v>
+      <c r="D335" s="19">
+        <v>0.73099999999999998</v>
       </c>
       <c r="E335" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F335" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G335" s="1" t="s">
         <v>282</v>
@@ -10696,8 +10522,8 @@
       </c>
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A336" s="1" t="s">
-        <v>333</v>
+      <c r="A336" s="19">
+        <v>9358</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>12</v>
@@ -10705,14 +10531,14 @@
       <c r="C336" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D336" s="1" t="s">
-        <v>334</v>
+      <c r="D336" s="19">
+        <v>7.351</v>
       </c>
       <c r="E336" s="1" t="s">
         <v>107</v>
       </c>
       <c r="F336" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G336" s="1" t="s">
         <v>281</v>
@@ -10722,8 +10548,8 @@
       </c>
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A337" s="1" t="s">
-        <v>335</v>
+      <c r="A337" s="19">
+        <v>9984</v>
       </c>
       <c r="B337" s="1" t="s">
         <v>11</v>
@@ -10731,14 +10557,14 @@
       <c r="C337" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D337" s="1" t="s">
-        <v>336</v>
+      <c r="D337" s="19">
+        <v>7.4039999999999999</v>
       </c>
       <c r="E337" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F337" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G337" s="1" t="s">
         <v>286</v>
@@ -10748,8 +10574,8 @@
       </c>
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A338" s="1" t="s">
-        <v>337</v>
+      <c r="A338" s="19">
+        <v>9999</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>27</v>
@@ -10757,14 +10583,14 @@
       <c r="C338" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D338" s="1" t="s">
-        <v>338</v>
+      <c r="D338" s="19">
+        <v>8.7319999999999993</v>
       </c>
       <c r="E338" s="1" t="s">
         <v>111</v>
       </c>
       <c r="F338" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G338" s="1" t="s">
         <v>281</v>
@@ -10774,23 +10600,23 @@
       </c>
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A339" s="1" t="s">
-        <v>339</v>
+      <c r="A339" s="19">
+        <v>10055</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>340</v>
+        <v>307</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D339" s="1" t="s">
-        <v>342</v>
+        <v>308</v>
+      </c>
+      <c r="D339" s="19">
+        <v>32.679000000000002</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F339" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G339" s="1" t="s">
         <v>282</v>
@@ -10800,23 +10626,23 @@
       </c>
     </row>
     <row r="340" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A340" s="1" t="s">
-        <v>343</v>
+      <c r="A340" s="19">
+        <v>10131</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>344</v>
+        <v>309</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D340" s="1" t="s">
-        <v>346</v>
+        <v>310</v>
+      </c>
+      <c r="D340" s="19">
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="E340" s="1" t="s">
         <v>200</v>
       </c>
       <c r="F340" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G340" s="1" t="s">
         <v>281</v>
@@ -10826,23 +10652,23 @@
       </c>
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A341" s="1" t="s">
-        <v>347</v>
+      <c r="A341" s="19">
+        <v>10124</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>348</v>
+        <v>311</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D341" s="1" t="s">
-        <v>350</v>
+        <v>312</v>
+      </c>
+      <c r="D341" s="19">
+        <v>28.260999999999999</v>
       </c>
       <c r="E341" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F341" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G341" s="1" t="s">
         <v>282</v>
@@ -10852,8 +10678,8 @@
       </c>
     </row>
     <row r="342" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A342" s="1" t="s">
-        <v>351</v>
+      <c r="A342" s="19">
+        <v>10114</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>253</v>
@@ -10861,14 +10687,14 @@
       <c r="C342" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D342" s="1" t="s">
-        <v>352</v>
+      <c r="D342" s="19">
+        <v>0.35</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="F342" s="12" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="G342" s="1" t="s">
         <v>282</v>
@@ -10878,8 +10704,8 @@
       </c>
     </row>
     <row r="343" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A343" s="1" t="s">
-        <v>307</v>
+      <c r="A343" s="19">
+        <v>10133</v>
       </c>
       <c r="B343" s="1" t="s">
         <v>275</v>
@@ -10887,14 +10713,14 @@
       <c r="C343" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D343" s="1" t="s">
-        <v>356</v>
+      <c r="D343" s="19">
+        <v>19.451000000000001</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="F343" s="20" t="s">
-        <v>377</v>
+      <c r="F343" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G343" s="2" t="s">
         <v>282</v>
@@ -10904,8 +10730,8 @@
       </c>
     </row>
     <row r="344" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A344" s="1" t="s">
-        <v>329</v>
+      <c r="A344" s="19">
+        <v>10137</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>277</v>
@@ -10913,14 +10739,14 @@
       <c r="C344" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D344" s="1" t="s">
-        <v>357</v>
+      <c r="D344" s="19">
+        <v>63.655000000000001</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F344" s="20" t="s">
-        <v>377</v>
+      <c r="F344" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G344" s="2" t="s">
         <v>282</v>
@@ -10930,8 +10756,8 @@
       </c>
     </row>
     <row r="345" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A345" s="1" t="s">
-        <v>315</v>
+      <c r="A345" s="19">
+        <v>9359</v>
       </c>
       <c r="B345" s="1" t="s">
         <v>30</v>
@@ -10939,14 +10765,14 @@
       <c r="C345" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D345" s="1" t="s">
-        <v>358</v>
+      <c r="D345" s="19">
+        <v>9.6809999999999992</v>
       </c>
       <c r="E345" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F345" s="20" t="s">
-        <v>377</v>
+      <c r="F345" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G345" s="2" t="s">
         <v>281</v>
@@ -10956,23 +10782,23 @@
       </c>
     </row>
     <row r="346" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A346" s="1" t="s">
-        <v>339</v>
+      <c r="A346" s="19">
+        <v>10055</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>340</v>
+        <v>307</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D346" s="1" t="s">
-        <v>359</v>
+        <v>308</v>
+      </c>
+      <c r="D346" s="19">
+        <v>61.058</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="F346" s="20" t="s">
-        <v>377</v>
+        <v>315</v>
+      </c>
+      <c r="F346" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G346" s="2" t="s">
         <v>282</v>
@@ -10982,8 +10808,8 @@
       </c>
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A347" s="1" t="s">
-        <v>327</v>
+      <c r="A347" s="19">
+        <v>10116</v>
       </c>
       <c r="B347" s="1" t="s">
         <v>248</v>
@@ -10991,14 +10817,14 @@
       <c r="C347" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D347" s="1" t="s">
-        <v>360</v>
+      <c r="D347" s="19">
+        <v>47.463000000000001</v>
       </c>
       <c r="E347" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F347" s="20" t="s">
-        <v>377</v>
+      <c r="F347" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G347" s="2" t="s">
         <v>282</v>
@@ -11008,23 +10834,23 @@
       </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A348" s="1" t="s">
-        <v>347</v>
+      <c r="A348" s="19">
+        <v>10124</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>348</v>
+        <v>311</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D348" s="1" t="s">
-        <v>361</v>
+        <v>312</v>
+      </c>
+      <c r="D348" s="19">
+        <v>41.618000000000002</v>
       </c>
       <c r="E348" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F348" s="20" t="s">
-        <v>377</v>
+      <c r="F348" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G348" s="2" t="s">
         <v>282</v>
@@ -11034,8 +10860,8 @@
       </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A349" s="1" t="s">
-        <v>311</v>
+      <c r="A349" s="19">
+        <v>10138</v>
       </c>
       <c r="B349" s="1" t="s">
         <v>269</v>
@@ -11043,14 +10869,14 @@
       <c r="C349" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D349" s="1" t="s">
-        <v>362</v>
+      <c r="D349" s="19">
+        <v>12.316000000000001</v>
       </c>
       <c r="E349" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F349" s="20" t="s">
-        <v>377</v>
+      <c r="F349" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G349" s="2" t="s">
         <v>282</v>
@@ -11060,23 +10886,23 @@
       </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A350" s="1" t="s">
-        <v>363</v>
+      <c r="A350" s="19">
+        <v>10140</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>364</v>
+        <v>316</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="D350" s="1" t="s">
-        <v>366</v>
+        <v>317</v>
+      </c>
+      <c r="D350" s="19">
+        <v>26.346</v>
       </c>
       <c r="E350" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="F350" s="20" t="s">
-        <v>377</v>
+      <c r="F350" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G350" s="2" t="s">
         <v>282</v>
@@ -11086,8 +10912,8 @@
       </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A351" s="1" t="s">
-        <v>317</v>
+      <c r="A351" s="19">
+        <v>9360</v>
       </c>
       <c r="B351" s="1" t="s">
         <v>0</v>
@@ -11095,14 +10921,14 @@
       <c r="C351" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D351" s="1" t="s">
-        <v>367</v>
+      <c r="D351" s="19">
+        <v>20.596</v>
       </c>
       <c r="E351" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F351" s="20" t="s">
-        <v>377</v>
+      <c r="F351" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G351" s="2" t="s">
         <v>281</v>
@@ -11112,8 +10938,8 @@
       </c>
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A352" s="1" t="s">
-        <v>333</v>
+      <c r="A352" s="19">
+        <v>9358</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>12</v>
@@ -11121,14 +10947,14 @@
       <c r="C352" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D352" s="1" t="s">
-        <v>368</v>
+      <c r="D352" s="19">
+        <v>10.041</v>
       </c>
       <c r="E352" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F352" s="20" t="s">
-        <v>377</v>
+      <c r="F352" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G352" s="2" t="s">
         <v>281</v>
@@ -11138,8 +10964,8 @@
       </c>
     </row>
     <row r="353" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A353" s="1" t="s">
-        <v>319</v>
+      <c r="A353" s="19">
+        <v>9361</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>21</v>
@@ -11147,14 +10973,14 @@
       <c r="C353" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D353" s="1" t="s">
-        <v>369</v>
+      <c r="D353" s="19">
+        <v>12.884</v>
       </c>
       <c r="E353" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F353" s="20" t="s">
-        <v>377</v>
+      <c r="F353" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G353" s="2" t="s">
         <v>281</v>
@@ -11164,8 +10990,8 @@
       </c>
     </row>
     <row r="354" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A354" s="1" t="s">
-        <v>335</v>
+      <c r="A354" s="19">
+        <v>9984</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>11</v>
@@ -11173,14 +10999,14 @@
       <c r="C354" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D354" s="1" t="s">
-        <v>370</v>
+      <c r="D354" s="19">
+        <v>8.173</v>
       </c>
       <c r="E354" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F354" s="20" t="s">
-        <v>377</v>
+      <c r="F354" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G354" s="2" t="s">
         <v>286</v>
@@ -11190,8 +11016,8 @@
       </c>
     </row>
     <row r="355" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A355" s="1" t="s">
-        <v>337</v>
+      <c r="A355" s="19">
+        <v>9999</v>
       </c>
       <c r="B355" s="1" t="s">
         <v>27</v>
@@ -11199,14 +11025,14 @@
       <c r="C355" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D355" s="1" t="s">
-        <v>371</v>
+      <c r="D355" s="19">
+        <v>7.548</v>
       </c>
       <c r="E355" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F355" s="20" t="s">
-        <v>377</v>
+      <c r="F355" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G355" s="2" t="s">
         <v>281</v>
@@ -11216,23 +11042,23 @@
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A356" s="1" t="s">
-        <v>372</v>
+      <c r="A356" s="19">
+        <v>10130</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>373</v>
+        <v>318</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D356" s="1" t="s">
-        <v>375</v>
+        <v>319</v>
+      </c>
+      <c r="D356" s="19">
+        <v>0.56499999999999995</v>
       </c>
       <c r="E356" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F356" s="20" t="s">
-        <v>377</v>
+      <c r="F356" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G356" s="2" t="s">
         <v>281</v>
@@ -11242,8 +11068,8 @@
       </c>
     </row>
     <row r="357" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A357" s="1" t="s">
-        <v>321</v>
+      <c r="A357" s="19">
+        <v>9364</v>
       </c>
       <c r="B357" s="1" t="s">
         <v>32</v>
@@ -11251,14 +11077,14 @@
       <c r="C357" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D357" s="1" t="s">
-        <v>376</v>
+      <c r="D357" s="19">
+        <v>0.20899999999999999</v>
       </c>
       <c r="E357" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F357" s="20" t="s">
-        <v>377</v>
+      <c r="F357" s="18" t="s">
+        <v>320</v>
       </c>
       <c r="G357" s="2" t="s">
         <v>281</v>
@@ -11269,33 +11095,33 @@
     </row>
     <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
-      <c r="B358" s="16"/>
-      <c r="C358" s="16"/>
-      <c r="D358" s="13"/>
+      <c r="B358" s="15"/>
+      <c r="C358" s="15"/>
+      <c r="D358" s="1"/>
       <c r="E358" s="1"/>
-      <c r="F358" s="14"/>
+      <c r="F358" s="13"/>
       <c r="G358" s="2"/>
-      <c r="H358" s="16"/>
+      <c r="H358" s="15"/>
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A359" s="1"/>
-      <c r="B359" s="16"/>
-      <c r="C359" s="16"/>
-      <c r="D359" s="13"/>
+      <c r="B359" s="15"/>
+      <c r="C359" s="15"/>
+      <c r="D359" s="1"/>
       <c r="E359" s="1"/>
-      <c r="F359" s="14"/>
+      <c r="F359" s="13"/>
       <c r="G359" s="2"/>
-      <c r="H359" s="16"/>
+      <c r="H359" s="15"/>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A360" s="15"/>
-      <c r="B360" s="16"/>
-      <c r="C360" s="16"/>
-      <c r="D360" s="17"/>
-      <c r="E360" s="15"/>
-      <c r="F360" s="18"/>
-      <c r="G360" s="19"/>
-      <c r="H360" s="16"/>
+      <c r="A360" s="14"/>
+      <c r="B360" s="15"/>
+      <c r="C360" s="15"/>
+      <c r="D360" s="14"/>
+      <c r="E360" s="14"/>
+      <c r="F360" s="16"/>
+      <c r="G360" s="17"/>
+      <c r="H360" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>